<commit_message>
adapt notebook & transformations
</commit_message>
<xml_diff>
--- a/ssp_modeling/scenario_mapping/ssp_mexico_transformation_cw.xlsx
+++ b/ssp_modeling/scenario_mapping/ssp_mexico_transformation_cw.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabianfuentes/Documents/git/ssp_egypt/ssp_modeling/scenario_mapping/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabianfuentes/git/ssp_mexico/ssp_modeling/scenario_mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC362B65-3D01-1A4B-BF79-697C68C39FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7236C0-6A48-884C-9CB4-51B07503BF3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-7140" windowWidth="38400" windowHeight="20980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="yaml" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">main!$A$1:$N$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$A$1:$O$62</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1">yaml!$A$1:$D$62</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="409">
   <si>
     <t>subsector</t>
   </si>
@@ -1308,6 +1308,9 @@
   </si>
   <si>
     <t>magnitude_description</t>
+  </si>
+  <si>
+    <t>strategy_NDC+</t>
   </si>
 </sst>
 </file>
@@ -1471,7 +1474,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1564,9 +1567,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1915,11 +1915,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:R65"/>
+  <dimension ref="A1:S65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1932,20 +1932,22 @@
     <col min="7" max="7" width="47.5" style="4" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="48.5" style="4" hidden="1" customWidth="1"/>
     <col min="9" max="10" width="35" style="4" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="31.5" style="39" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.83203125" style="38" customWidth="1"/>
-    <col min="13" max="14" width="20.5" style="40" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.5" style="41" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5" style="42" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.5" style="40" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.5" style="43" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.5" style="38" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.83203125" style="37" customWidth="1"/>
+    <col min="13" max="13" width="20.5" style="39" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.5" style="39" customWidth="1"/>
+    <col min="15" max="15" width="20.5" style="39" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5" style="40" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5" style="41" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.5" style="39" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.5" style="42" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="4" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="4" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -1982,14 +1984,17 @@
         <v>208</v>
       </c>
       <c r="N1" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="O1" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="O1" s="10"/>
       <c r="P1" s="10"/>
-      <c r="Q1" s="11"/>
+      <c r="Q1" s="10"/>
       <c r="R1" s="11"/>
-    </row>
-    <row r="2" spans="1:18" s="4" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S1" s="11"/>
+    </row>
+    <row r="2" spans="1:19" s="4" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>210</v>
       </c>
@@ -2019,19 +2024,20 @@
         <v>12</v>
       </c>
       <c r="M2" s="16"/>
-      <c r="N2" s="16">
-        <v>1</v>
-      </c>
-      <c r="O2" s="10"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16">
+        <v>1</v>
+      </c>
       <c r="P2" s="10"/>
-      <c r="Q2" s="11"/>
+      <c r="Q2" s="10"/>
       <c r="R2" s="11"/>
-    </row>
-    <row r="3" spans="1:18" s="4" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S2" s="11"/>
+    </row>
+    <row r="3" spans="1:19" s="4" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="44" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="17" t="s">
@@ -2057,15 +2063,16 @@
         <v>12</v>
       </c>
       <c r="M3" s="16"/>
-      <c r="N3" s="16">
-        <v>1</v>
-      </c>
-      <c r="O3" s="10"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16">
+        <v>1</v>
+      </c>
       <c r="P3" s="10"/>
-      <c r="Q3" s="11"/>
+      <c r="Q3" s="10"/>
       <c r="R3" s="11"/>
-    </row>
-    <row r="4" spans="1:18" s="4" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S3" s="11"/>
+    </row>
+    <row r="4" spans="1:19" s="4" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>210</v>
       </c>
@@ -2095,15 +2102,16 @@
         <v>12</v>
       </c>
       <c r="M4" s="16"/>
-      <c r="N4" s="16">
-        <v>1</v>
-      </c>
-      <c r="O4" s="10"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16">
+        <v>1</v>
+      </c>
       <c r="P4" s="10"/>
-      <c r="Q4" s="11"/>
+      <c r="Q4" s="10"/>
       <c r="R4" s="11"/>
-    </row>
-    <row r="5" spans="1:18" s="4" customFormat="1" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S4" s="11"/>
+    </row>
+    <row r="5" spans="1:19" s="4" customFormat="1" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>210</v>
       </c>
@@ -2138,12 +2146,15 @@
       <c r="N5" s="16">
         <v>1</v>
       </c>
-      <c r="O5" s="10"/>
+      <c r="O5" s="16">
+        <v>1</v>
+      </c>
       <c r="P5" s="10"/>
-      <c r="Q5" s="11"/>
+      <c r="Q5" s="10"/>
       <c r="R5" s="11"/>
-    </row>
-    <row r="6" spans="1:18" s="4" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S5" s="11"/>
+    </row>
+    <row r="6" spans="1:19" s="4" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>210</v>
       </c>
@@ -2177,15 +2188,14 @@
         <v>12</v>
       </c>
       <c r="M6" s="16"/>
-      <c r="N6" s="16">
-        <v>1</v>
-      </c>
-      <c r="O6" s="10"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
       <c r="P6" s="10"/>
-      <c r="Q6" s="11"/>
+      <c r="Q6" s="10"/>
       <c r="R6" s="11"/>
-    </row>
-    <row r="7" spans="1:18" s="4" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S6" s="11"/>
+    </row>
+    <row r="7" spans="1:19" s="4" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
         <v>224</v>
       </c>
@@ -2215,15 +2225,18 @@
         <v>12</v>
       </c>
       <c r="M7" s="16"/>
-      <c r="N7" s="46">
+      <c r="N7" s="16">
+        <v>0.05</v>
+      </c>
+      <c r="O7" s="45">
         <v>0.1</v>
       </c>
-      <c r="O7" s="10"/>
       <c r="P7" s="10"/>
-      <c r="Q7" s="11"/>
+      <c r="Q7" s="10"/>
       <c r="R7" s="11"/>
-    </row>
-    <row r="8" spans="1:18" s="4" customFormat="1" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S7" s="11"/>
+    </row>
+    <row r="8" spans="1:19" s="4" customFormat="1" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>224</v>
       </c>
@@ -2257,15 +2270,16 @@
         <v>12</v>
       </c>
       <c r="M8" s="16"/>
-      <c r="N8" s="16">
-        <v>1</v>
-      </c>
-      <c r="O8" s="10"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16">
+        <v>1</v>
+      </c>
       <c r="P8" s="10"/>
-      <c r="Q8" s="11"/>
+      <c r="Q8" s="10"/>
       <c r="R8" s="11"/>
-    </row>
-    <row r="9" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S8" s="11"/>
+    </row>
+    <row r="9" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>224</v>
       </c>
@@ -2299,15 +2313,16 @@
         <v>12</v>
       </c>
       <c r="M9" s="16"/>
-      <c r="N9" s="16">
-        <v>1</v>
-      </c>
-      <c r="O9" s="10"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16">
+        <v>1</v>
+      </c>
       <c r="P9" s="10"/>
-      <c r="Q9" s="11"/>
+      <c r="Q9" s="10"/>
       <c r="R9" s="11"/>
-    </row>
-    <row r="10" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S9" s="11"/>
+    </row>
+    <row r="10" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>224</v>
       </c>
@@ -2341,15 +2356,16 @@
         <v>12</v>
       </c>
       <c r="M10" s="16"/>
-      <c r="N10" s="16">
-        <v>1</v>
-      </c>
-      <c r="O10" s="10"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16">
+        <v>1</v>
+      </c>
       <c r="P10" s="10"/>
-      <c r="Q10" s="11"/>
+      <c r="Q10" s="10"/>
       <c r="R10" s="11"/>
-    </row>
-    <row r="11" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S10" s="11"/>
+    </row>
+    <row r="11" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>224</v>
       </c>
@@ -2382,12 +2398,15 @@
       <c r="N11" s="16">
         <v>1</v>
       </c>
-      <c r="O11" s="10"/>
+      <c r="O11" s="16">
+        <v>1</v>
+      </c>
       <c r="P11" s="10"/>
-      <c r="Q11" s="11"/>
+      <c r="Q11" s="10"/>
       <c r="R11" s="11"/>
-    </row>
-    <row r="12" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S11" s="11"/>
+    </row>
+    <row r="12" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>224</v>
       </c>
@@ -2420,12 +2439,15 @@
       <c r="N12" s="16">
         <v>1</v>
       </c>
-      <c r="O12" s="10"/>
+      <c r="O12" s="16">
+        <v>1</v>
+      </c>
       <c r="P12" s="10"/>
-      <c r="Q12" s="11"/>
+      <c r="Q12" s="10"/>
       <c r="R12" s="11"/>
-    </row>
-    <row r="13" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S12" s="11"/>
+    </row>
+    <row r="13" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>224</v>
       </c>
@@ -2464,12 +2486,15 @@
       <c r="N13" s="16">
         <v>1</v>
       </c>
-      <c r="O13" s="10"/>
+      <c r="O13" s="16">
+        <v>1</v>
+      </c>
       <c r="P13" s="10"/>
-      <c r="Q13" s="11"/>
+      <c r="Q13" s="10"/>
       <c r="R13" s="11"/>
-    </row>
-    <row r="14" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S13" s="11"/>
+    </row>
+    <row r="14" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>224</v>
       </c>
@@ -2503,15 +2528,16 @@
         <v>12</v>
       </c>
       <c r="M14" s="16"/>
-      <c r="N14" s="16">
-        <v>1</v>
-      </c>
-      <c r="O14" s="10"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16">
+        <v>1</v>
+      </c>
       <c r="P14" s="10"/>
-      <c r="Q14" s="11"/>
+      <c r="Q14" s="10"/>
       <c r="R14" s="11"/>
-    </row>
-    <row r="15" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S14" s="11"/>
+    </row>
+    <row r="15" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
         <v>224</v>
       </c>
@@ -2541,15 +2567,16 @@
         <v>12</v>
       </c>
       <c r="M15" s="16"/>
-      <c r="N15" s="16">
-        <v>1</v>
-      </c>
-      <c r="O15" s="10"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16">
+        <v>1</v>
+      </c>
       <c r="P15" s="10"/>
-      <c r="Q15" s="11"/>
+      <c r="Q15" s="10"/>
       <c r="R15" s="11"/>
-    </row>
-    <row r="16" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S15" s="11"/>
+    </row>
+    <row r="16" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>51</v>
       </c>
@@ -2583,15 +2610,16 @@
         <v>12</v>
       </c>
       <c r="M16" s="16"/>
-      <c r="N16" s="16">
-        <v>1</v>
-      </c>
-      <c r="O16" s="10"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16">
+        <v>1</v>
+      </c>
       <c r="P16" s="10"/>
-      <c r="Q16" s="11"/>
+      <c r="Q16" s="10"/>
       <c r="R16" s="11"/>
-    </row>
-    <row r="17" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S16" s="11"/>
+    </row>
+    <row r="17" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>51</v>
       </c>
@@ -2625,15 +2653,16 @@
         <v>12</v>
       </c>
       <c r="M17" s="16"/>
-      <c r="N17" s="16">
-        <v>1</v>
-      </c>
-      <c r="O17" s="10"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16">
+        <v>1</v>
+      </c>
       <c r="P17" s="10"/>
-      <c r="Q17" s="11"/>
+      <c r="Q17" s="10"/>
       <c r="R17" s="11"/>
-    </row>
-    <row r="18" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S17" s="11"/>
+    </row>
+    <row r="18" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>51</v>
       </c>
@@ -2667,15 +2696,16 @@
         <v>12</v>
       </c>
       <c r="M18" s="16"/>
-      <c r="N18" s="16">
-        <v>1</v>
-      </c>
-      <c r="O18" s="10"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16">
+        <v>1</v>
+      </c>
       <c r="P18" s="10"/>
-      <c r="Q18" s="11"/>
+      <c r="Q18" s="10"/>
       <c r="R18" s="11"/>
-    </row>
-    <row r="19" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S18" s="11"/>
+    </row>
+    <row r="19" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>51</v>
       </c>
@@ -2705,15 +2735,16 @@
         <v>12</v>
       </c>
       <c r="M19" s="16"/>
-      <c r="N19" s="16">
-        <v>1</v>
-      </c>
-      <c r="O19" s="10"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16">
+        <v>1</v>
+      </c>
       <c r="P19" s="10"/>
-      <c r="Q19" s="11"/>
+      <c r="Q19" s="10"/>
       <c r="R19" s="11"/>
-    </row>
-    <row r="20" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S19" s="11"/>
+    </row>
+    <row r="20" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>51</v>
       </c>
@@ -2743,15 +2774,16 @@
         <v>12</v>
       </c>
       <c r="M20" s="16"/>
-      <c r="N20" s="16">
-        <v>1</v>
-      </c>
-      <c r="O20" s="10"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16">
+        <v>1</v>
+      </c>
       <c r="P20" s="10"/>
-      <c r="Q20" s="11"/>
+      <c r="Q20" s="10"/>
       <c r="R20" s="11"/>
-    </row>
-    <row r="21" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S20" s="11"/>
+    </row>
+    <row r="21" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>51</v>
       </c>
@@ -2781,15 +2813,16 @@
         <v>12</v>
       </c>
       <c r="M21" s="16"/>
-      <c r="N21" s="16">
-        <v>1</v>
-      </c>
-      <c r="O21" s="10"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16">
+        <v>1</v>
+      </c>
       <c r="P21" s="10"/>
-      <c r="Q21" s="11"/>
+      <c r="Q21" s="10"/>
       <c r="R21" s="11"/>
-    </row>
-    <row r="22" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S21" s="11"/>
+    </row>
+    <row r="22" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>210</v>
       </c>
@@ -2823,17 +2856,20 @@
         <v>12</v>
       </c>
       <c r="M22" s="16">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N22" s="16">
         <v>1</v>
       </c>
-      <c r="O22" s="10"/>
+      <c r="O22" s="16">
+        <v>1</v>
+      </c>
       <c r="P22" s="10"/>
-      <c r="Q22" s="11"/>
+      <c r="Q22" s="10"/>
       <c r="R22" s="11"/>
-    </row>
-    <row r="23" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S22" s="11"/>
+    </row>
+    <row r="23" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>210</v>
       </c>
@@ -2868,12 +2904,13 @@
       </c>
       <c r="M23" s="16"/>
       <c r="N23" s="16"/>
-      <c r="O23" s="10"/>
+      <c r="O23" s="16"/>
       <c r="P23" s="10"/>
-      <c r="Q23" s="11"/>
+      <c r="Q23" s="10"/>
       <c r="R23" s="11"/>
-    </row>
-    <row r="24" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S23" s="11"/>
+    </row>
+    <row r="24" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>210</v>
       </c>
@@ -2907,17 +2944,20 @@
         <v>12</v>
       </c>
       <c r="M24" s="16">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N24" s="16">
-        <v>2</v>
-      </c>
-      <c r="O24" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="O24" s="16">
+        <v>1</v>
+      </c>
       <c r="P24" s="10"/>
-      <c r="Q24" s="11"/>
+      <c r="Q24" s="10"/>
       <c r="R24" s="11"/>
-    </row>
-    <row r="25" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S24" s="11"/>
+    </row>
+    <row r="25" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>210</v>
       </c>
@@ -2952,12 +2992,13 @@
       </c>
       <c r="M25" s="16"/>
       <c r="N25" s="16"/>
-      <c r="O25" s="10"/>
+      <c r="O25" s="16"/>
       <c r="P25" s="10"/>
-      <c r="Q25" s="11"/>
+      <c r="Q25" s="10"/>
       <c r="R25" s="11"/>
-    </row>
-    <row r="26" spans="1:18" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S25" s="11"/>
+    </row>
+    <row r="26" spans="1:19" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
         <v>210</v>
       </c>
@@ -2987,15 +3028,16 @@
         <v>12</v>
       </c>
       <c r="M26" s="16"/>
-      <c r="N26" s="16">
-        <v>1.05</v>
-      </c>
-      <c r="O26" s="28"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="16">
+        <v>1</v>
+      </c>
       <c r="P26" s="28"/>
-      <c r="Q26" s="29"/>
-      <c r="R26" s="30"/>
-    </row>
-    <row r="27" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q26" s="28"/>
+      <c r="R26" s="29"/>
+      <c r="S26" s="30"/>
+    </row>
+    <row r="27" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>210</v>
       </c>
@@ -3025,15 +3067,16 @@
         <v>12</v>
       </c>
       <c r="M27" s="16"/>
-      <c r="N27" s="16">
-        <v>1</v>
-      </c>
-      <c r="O27" s="10"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16">
+        <v>1</v>
+      </c>
       <c r="P27" s="10"/>
-      <c r="Q27" s="11"/>
+      <c r="Q27" s="10"/>
       <c r="R27" s="11"/>
-    </row>
-    <row r="28" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S27" s="11"/>
+    </row>
+    <row r="28" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>210</v>
       </c>
@@ -3063,15 +3106,16 @@
         <v>12</v>
       </c>
       <c r="M28" s="16"/>
-      <c r="N28" s="16">
-        <v>1</v>
-      </c>
-      <c r="O28" s="10"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="16">
+        <v>1</v>
+      </c>
       <c r="P28" s="10"/>
-      <c r="Q28" s="11"/>
+      <c r="Q28" s="10"/>
       <c r="R28" s="11"/>
-    </row>
-    <row r="29" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S28" s="11"/>
+    </row>
+    <row r="29" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>210</v>
       </c>
@@ -3101,15 +3145,16 @@
         <v>12</v>
       </c>
       <c r="M29" s="16"/>
-      <c r="N29" s="16">
-        <v>1</v>
-      </c>
-      <c r="O29" s="10"/>
+      <c r="N29" s="16"/>
+      <c r="O29" s="16">
+        <v>1</v>
+      </c>
       <c r="P29" s="10"/>
-      <c r="Q29" s="11"/>
+      <c r="Q29" s="10"/>
       <c r="R29" s="11"/>
-    </row>
-    <row r="30" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S29" s="11"/>
+    </row>
+    <row r="30" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>210</v>
       </c>
@@ -3139,15 +3184,16 @@
         <v>12</v>
       </c>
       <c r="M30" s="16"/>
-      <c r="N30" s="16">
-        <v>1</v>
-      </c>
-      <c r="O30" s="10"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="16">
+        <v>1</v>
+      </c>
       <c r="P30" s="10"/>
-      <c r="Q30" s="11"/>
+      <c r="Q30" s="10"/>
       <c r="R30" s="11"/>
-    </row>
-    <row r="31" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S30" s="11"/>
+    </row>
+    <row r="31" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>210</v>
       </c>
@@ -3177,15 +3223,16 @@
         <v>12</v>
       </c>
       <c r="M31" s="16"/>
-      <c r="N31" s="16">
-        <v>1</v>
-      </c>
-      <c r="O31" s="10"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="16">
+        <v>1</v>
+      </c>
       <c r="P31" s="10"/>
-      <c r="Q31" s="11"/>
+      <c r="Q31" s="10"/>
       <c r="R31" s="11"/>
-    </row>
-    <row r="32" spans="1:18" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S31" s="11"/>
+    </row>
+    <row r="32" spans="1:19" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
         <v>210</v>
       </c>
@@ -3219,15 +3266,14 @@
         <v>12</v>
       </c>
       <c r="M32" s="16"/>
-      <c r="N32" s="16">
-        <v>0.7</v>
-      </c>
-      <c r="O32" s="31"/>
-      <c r="P32" s="28"/>
-      <c r="Q32" s="16"/>
-      <c r="R32" s="32"/>
-    </row>
-    <row r="33" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N32" s="16"/>
+      <c r="O32" s="16"/>
+      <c r="P32" s="31"/>
+      <c r="Q32" s="28"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="11"/>
+    </row>
+    <row r="33" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>307</v>
       </c>
@@ -3258,12 +3304,13 @@
       </c>
       <c r="M33" s="16"/>
       <c r="N33" s="16"/>
-      <c r="O33" s="10"/>
+      <c r="O33" s="16"/>
       <c r="P33" s="10"/>
-      <c r="Q33" s="11"/>
+      <c r="Q33" s="10"/>
       <c r="R33" s="11"/>
-    </row>
-    <row r="34" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S33" s="11"/>
+    </row>
+    <row r="34" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>307</v>
       </c>
@@ -3293,15 +3340,16 @@
         <v>12</v>
       </c>
       <c r="M34" s="16"/>
-      <c r="N34" s="16">
-        <v>1</v>
-      </c>
-      <c r="O34" s="10"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16">
+        <v>1</v>
+      </c>
       <c r="P34" s="10"/>
-      <c r="Q34" s="11"/>
+      <c r="Q34" s="10"/>
       <c r="R34" s="11"/>
-    </row>
-    <row r="35" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S34" s="11"/>
+    </row>
+    <row r="35" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
         <v>224</v>
       </c>
@@ -3331,15 +3379,16 @@
         <v>12</v>
       </c>
       <c r="M35" s="16"/>
-      <c r="N35" s="16">
-        <v>1</v>
-      </c>
-      <c r="O35" s="10"/>
+      <c r="N35" s="16"/>
+      <c r="O35" s="16">
+        <v>1</v>
+      </c>
       <c r="P35" s="10"/>
-      <c r="Q35" s="11"/>
+      <c r="Q35" s="10"/>
       <c r="R35" s="11"/>
-    </row>
-    <row r="36" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S35" s="11"/>
+    </row>
+    <row r="36" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
         <v>224</v>
       </c>
@@ -3368,18 +3417,19 @@
       <c r="L36" s="13">
         <v>12</v>
       </c>
-      <c r="M36" s="16">
-        <v>1</v>
-      </c>
+      <c r="M36" s="16"/>
       <c r="N36" s="16">
         <v>1</v>
       </c>
-      <c r="O36" s="10"/>
+      <c r="O36" s="16">
+        <v>1</v>
+      </c>
       <c r="P36" s="10"/>
-      <c r="Q36" s="11"/>
+      <c r="Q36" s="10"/>
       <c r="R36" s="11"/>
-    </row>
-    <row r="37" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S36" s="11"/>
+    </row>
+    <row r="37" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="s">
         <v>224</v>
       </c>
@@ -3409,15 +3459,16 @@
         <v>12</v>
       </c>
       <c r="M37" s="16"/>
-      <c r="N37" s="16">
-        <v>1</v>
-      </c>
-      <c r="O37" s="10"/>
+      <c r="N37" s="16"/>
+      <c r="O37" s="16">
+        <v>1</v>
+      </c>
       <c r="P37" s="10"/>
-      <c r="Q37" s="11"/>
+      <c r="Q37" s="10"/>
       <c r="R37" s="11"/>
-    </row>
-    <row r="38" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S37" s="11"/>
+    </row>
+    <row r="38" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
         <v>210</v>
       </c>
@@ -3447,15 +3498,16 @@
         <v>12</v>
       </c>
       <c r="M38" s="16"/>
-      <c r="N38" s="16">
-        <v>1</v>
-      </c>
-      <c r="O38" s="10"/>
+      <c r="N38" s="16"/>
+      <c r="O38" s="16">
+        <v>1</v>
+      </c>
       <c r="P38" s="10"/>
-      <c r="Q38" s="11"/>
+      <c r="Q38" s="10"/>
       <c r="R38" s="11"/>
-    </row>
-    <row r="39" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S38" s="11"/>
+    </row>
+    <row r="39" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
         <v>210</v>
       </c>
@@ -3490,12 +3542,15 @@
       <c r="N39" s="16">
         <v>1</v>
       </c>
-      <c r="O39" s="10"/>
+      <c r="O39" s="16">
+        <v>1</v>
+      </c>
       <c r="P39" s="10"/>
-      <c r="Q39" s="11"/>
+      <c r="Q39" s="10"/>
       <c r="R39" s="11"/>
-    </row>
-    <row r="40" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S39" s="11"/>
+    </row>
+    <row r="40" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
         <v>224</v>
       </c>
@@ -3528,18 +3583,19 @@
       <c r="L40" s="13">
         <v>12</v>
       </c>
-      <c r="M40" s="16">
-        <v>1</v>
-      </c>
+      <c r="M40" s="16"/>
       <c r="N40" s="16">
-        <v>2</v>
-      </c>
-      <c r="O40" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="O40" s="16">
+        <v>1</v>
+      </c>
       <c r="P40" s="10"/>
-      <c r="Q40" s="11"/>
+      <c r="Q40" s="10"/>
       <c r="R40" s="11"/>
-    </row>
-    <row r="41" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S40" s="11"/>
+    </row>
+    <row r="41" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
         <v>224</v>
       </c>
@@ -3559,7 +3615,7 @@
         <v>327</v>
       </c>
       <c r="G41" s="12"/>
-      <c r="H41" s="33"/>
+      <c r="H41" s="32"/>
       <c r="I41" s="12" t="s">
         <v>328</v>
       </c>
@@ -3573,15 +3629,16 @@
         <v>12</v>
       </c>
       <c r="M41" s="16"/>
-      <c r="N41" s="16">
-        <v>2</v>
-      </c>
-      <c r="O41" s="10"/>
+      <c r="N41" s="16"/>
+      <c r="O41" s="16">
+        <v>1</v>
+      </c>
       <c r="P41" s="10"/>
-      <c r="Q41" s="11"/>
+      <c r="Q41" s="10"/>
       <c r="R41" s="11"/>
-    </row>
-    <row r="42" spans="1:18" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S41" s="11"/>
+    </row>
+    <row r="42" spans="1:19" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="12" t="s">
         <v>224</v>
       </c>
@@ -3601,7 +3658,7 @@
         <v>331</v>
       </c>
       <c r="G42" s="12"/>
-      <c r="H42" s="33"/>
+      <c r="H42" s="32"/>
       <c r="I42" s="12" t="s">
         <v>332</v>
       </c>
@@ -3615,15 +3672,16 @@
         <v>12</v>
       </c>
       <c r="M42" s="16"/>
-      <c r="N42" s="16">
-        <v>2</v>
-      </c>
-      <c r="O42" s="10"/>
+      <c r="N42" s="16"/>
+      <c r="O42" s="16">
+        <v>1</v>
+      </c>
       <c r="P42" s="10"/>
-      <c r="Q42" s="11"/>
+      <c r="Q42" s="10"/>
       <c r="R42" s="11"/>
-    </row>
-    <row r="43" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S42" s="11"/>
+    </row>
+    <row r="43" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
         <v>224</v>
       </c>
@@ -3653,15 +3711,16 @@
         <v>12</v>
       </c>
       <c r="M43" s="16"/>
-      <c r="N43" s="16">
-        <v>1</v>
-      </c>
-      <c r="O43" s="10"/>
+      <c r="N43" s="16"/>
+      <c r="O43" s="16">
+        <v>1</v>
+      </c>
       <c r="P43" s="10"/>
-      <c r="Q43" s="11"/>
+      <c r="Q43" s="10"/>
       <c r="R43" s="11"/>
-    </row>
-    <row r="44" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S43" s="11"/>
+    </row>
+    <row r="44" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="s">
         <v>224</v>
       </c>
@@ -3696,12 +3755,15 @@
       <c r="N44" s="16">
         <v>1</v>
       </c>
-      <c r="O44" s="10"/>
+      <c r="O44" s="16">
+        <v>1</v>
+      </c>
       <c r="P44" s="10"/>
-      <c r="Q44" s="11"/>
+      <c r="Q44" s="10"/>
       <c r="R44" s="11"/>
-    </row>
-    <row r="45" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S44" s="11"/>
+    </row>
+    <row r="45" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="12" t="s">
         <v>224</v>
       </c>
@@ -3735,15 +3797,16 @@
         <v>12</v>
       </c>
       <c r="M45" s="16"/>
-      <c r="N45" s="16">
-        <v>2</v>
-      </c>
-      <c r="O45" s="10"/>
+      <c r="N45" s="16"/>
+      <c r="O45" s="16">
+        <v>1</v>
+      </c>
       <c r="P45" s="10"/>
-      <c r="Q45" s="11"/>
+      <c r="Q45" s="10"/>
       <c r="R45" s="11"/>
-    </row>
-    <row r="46" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S45" s="11"/>
+    </row>
+    <row r="46" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="12" t="s">
         <v>224</v>
       </c>
@@ -3780,14 +3843,17 @@
         <v>1</v>
       </c>
       <c r="N46" s="16">
-        <v>2</v>
-      </c>
-      <c r="O46" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="O46" s="16">
+        <v>1</v>
+      </c>
       <c r="P46" s="10"/>
-      <c r="Q46" s="11"/>
+      <c r="Q46" s="10"/>
       <c r="R46" s="11"/>
-    </row>
-    <row r="47" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S46" s="11"/>
+    </row>
+    <row r="47" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="12" t="s">
         <v>224</v>
       </c>
@@ -3822,12 +3888,15 @@
       <c r="N47" s="16">
         <v>1</v>
       </c>
-      <c r="O47" s="10"/>
+      <c r="O47" s="16">
+        <v>1</v>
+      </c>
       <c r="P47" s="10"/>
-      <c r="Q47" s="11"/>
+      <c r="Q47" s="10"/>
       <c r="R47" s="11"/>
-    </row>
-    <row r="48" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S47" s="11"/>
+    </row>
+    <row r="48" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="12" t="s">
         <v>224</v>
       </c>
@@ -3864,14 +3933,17 @@
         <v>1</v>
       </c>
       <c r="N48" s="16">
-        <v>2</v>
-      </c>
-      <c r="O48" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="O48" s="16">
+        <v>1</v>
+      </c>
       <c r="P48" s="10"/>
-      <c r="Q48" s="11"/>
+      <c r="Q48" s="10"/>
       <c r="R48" s="11"/>
-    </row>
-    <row r="49" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S48" s="11"/>
+    </row>
+    <row r="49" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="12" t="s">
         <v>224</v>
       </c>
@@ -3908,14 +3980,17 @@
         <v>1</v>
       </c>
       <c r="N49" s="16">
-        <v>2</v>
-      </c>
-      <c r="O49" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="O49" s="16">
+        <v>1</v>
+      </c>
       <c r="P49" s="10"/>
-      <c r="Q49" s="11"/>
+      <c r="Q49" s="10"/>
       <c r="R49" s="11"/>
-    </row>
-    <row r="50" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S49" s="11"/>
+    </row>
+    <row r="50" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="12" t="s">
         <v>224</v>
       </c>
@@ -3949,15 +4024,16 @@
         <v>12</v>
       </c>
       <c r="M50" s="16"/>
-      <c r="N50" s="16">
-        <v>1</v>
-      </c>
-      <c r="O50" s="10"/>
+      <c r="N50" s="16"/>
+      <c r="O50" s="16">
+        <v>1</v>
+      </c>
       <c r="P50" s="10"/>
-      <c r="Q50" s="11"/>
+      <c r="Q50" s="10"/>
       <c r="R50" s="11"/>
-    </row>
-    <row r="51" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S50" s="11"/>
+    </row>
+    <row r="51" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="12" t="s">
         <v>51</v>
       </c>
@@ -3987,15 +4063,16 @@
         <v>12</v>
       </c>
       <c r="M51" s="16"/>
-      <c r="N51" s="16">
-        <v>1</v>
-      </c>
-      <c r="O51" s="10"/>
+      <c r="N51" s="16"/>
+      <c r="O51" s="16">
+        <v>1</v>
+      </c>
       <c r="P51" s="10"/>
-      <c r="Q51" s="11"/>
+      <c r="Q51" s="10"/>
       <c r="R51" s="11"/>
-    </row>
-    <row r="52" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S51" s="11"/>
+    </row>
+    <row r="52" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="12" t="s">
         <v>51</v>
       </c>
@@ -4029,15 +4106,16 @@
         <v>12</v>
       </c>
       <c r="M52" s="16"/>
-      <c r="N52" s="16">
-        <v>1</v>
-      </c>
-      <c r="O52" s="10"/>
+      <c r="N52" s="16"/>
+      <c r="O52" s="16">
+        <v>1</v>
+      </c>
       <c r="P52" s="10"/>
-      <c r="Q52" s="11"/>
+      <c r="Q52" s="10"/>
       <c r="R52" s="11"/>
-    </row>
-    <row r="53" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S52" s="11"/>
+    </row>
+    <row r="53" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="12" t="s">
         <v>367</v>
       </c>
@@ -4071,15 +4149,16 @@
         <v>12</v>
       </c>
       <c r="M53" s="16"/>
-      <c r="N53" s="16">
-        <v>2</v>
-      </c>
-      <c r="O53" s="10"/>
+      <c r="N53" s="16"/>
+      <c r="O53" s="16">
+        <v>1</v>
+      </c>
       <c r="P53" s="10"/>
-      <c r="Q53" s="11"/>
+      <c r="Q53" s="10"/>
       <c r="R53" s="11"/>
-    </row>
-    <row r="54" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S53" s="11"/>
+    </row>
+    <row r="54" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="12" t="s">
         <v>367</v>
       </c>
@@ -4113,15 +4192,16 @@
         <v>12</v>
       </c>
       <c r="M54" s="16"/>
-      <c r="N54" s="16">
-        <v>2</v>
-      </c>
-      <c r="O54" s="10"/>
+      <c r="N54" s="16"/>
+      <c r="O54" s="16">
+        <v>1</v>
+      </c>
       <c r="P54" s="10"/>
-      <c r="Q54" s="11"/>
+      <c r="Q54" s="10"/>
       <c r="R54" s="11"/>
-    </row>
-    <row r="55" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S54" s="11"/>
+    </row>
+    <row r="55" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="12" t="s">
         <v>367</v>
       </c>
@@ -4155,15 +4235,16 @@
         <v>12</v>
       </c>
       <c r="M55" s="16"/>
-      <c r="N55" s="16">
-        <v>2</v>
-      </c>
-      <c r="O55" s="10"/>
+      <c r="N55" s="16"/>
+      <c r="O55" s="16">
+        <v>1</v>
+      </c>
       <c r="P55" s="10"/>
-      <c r="Q55" s="11"/>
+      <c r="Q55" s="10"/>
       <c r="R55" s="11"/>
-    </row>
-    <row r="56" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S55" s="11"/>
+    </row>
+    <row r="56" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="12" t="s">
         <v>367</v>
       </c>
@@ -4197,15 +4278,16 @@
         <v>12</v>
       </c>
       <c r="M56" s="16"/>
-      <c r="N56" s="16">
-        <v>2</v>
-      </c>
-      <c r="O56" s="10"/>
+      <c r="N56" s="16"/>
+      <c r="O56" s="16">
+        <v>1</v>
+      </c>
       <c r="P56" s="10"/>
-      <c r="Q56" s="11"/>
+      <c r="Q56" s="10"/>
       <c r="R56" s="11"/>
-    </row>
-    <row r="57" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S56" s="11"/>
+    </row>
+    <row r="57" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="12" t="s">
         <v>367</v>
       </c>
@@ -4235,15 +4317,16 @@
         <v>12</v>
       </c>
       <c r="M57" s="16"/>
-      <c r="N57" s="16">
-        <v>1</v>
-      </c>
-      <c r="O57" s="10"/>
+      <c r="N57" s="16"/>
+      <c r="O57" s="16">
+        <v>1</v>
+      </c>
       <c r="P57" s="10"/>
-      <c r="Q57" s="11"/>
+      <c r="Q57" s="10"/>
       <c r="R57" s="11"/>
-    </row>
-    <row r="58" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S57" s="11"/>
+    </row>
+    <row r="58" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="12" t="s">
         <v>367</v>
       </c>
@@ -4277,15 +4360,16 @@
         <v>12</v>
       </c>
       <c r="M58" s="16"/>
-      <c r="N58" s="16">
-        <v>2</v>
-      </c>
-      <c r="O58" s="10"/>
+      <c r="N58" s="16"/>
+      <c r="O58" s="16">
+        <v>1</v>
+      </c>
       <c r="P58" s="10"/>
-      <c r="Q58" s="11"/>
+      <c r="Q58" s="10"/>
       <c r="R58" s="11"/>
-    </row>
-    <row r="59" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S58" s="11"/>
+    </row>
+    <row r="59" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="12" t="s">
         <v>367</v>
       </c>
@@ -4315,15 +4399,16 @@
         <v>12</v>
       </c>
       <c r="M59" s="16"/>
-      <c r="N59" s="16">
-        <v>2</v>
-      </c>
-      <c r="O59" s="10"/>
+      <c r="N59" s="16"/>
+      <c r="O59" s="16">
+        <v>1</v>
+      </c>
       <c r="P59" s="10"/>
-      <c r="Q59" s="11"/>
-      <c r="R59" s="11"/>
-    </row>
-    <row r="60" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q59" s="10"/>
+      <c r="R59" s="29"/>
+      <c r="S59" s="30"/>
+    </row>
+    <row r="60" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="12" t="s">
         <v>367</v>
       </c>
@@ -4353,15 +4438,16 @@
         <v>12</v>
       </c>
       <c r="M60" s="16"/>
-      <c r="N60" s="16">
-        <v>2</v>
-      </c>
-      <c r="O60" s="10"/>
+      <c r="N60" s="16"/>
+      <c r="O60" s="16">
+        <v>1</v>
+      </c>
       <c r="P60" s="10"/>
-      <c r="Q60" s="11"/>
-      <c r="R60" s="11"/>
-    </row>
-    <row r="61" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q60" s="10"/>
+      <c r="R60" s="29"/>
+      <c r="S60" s="30"/>
+    </row>
+    <row r="61" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="12" t="s">
         <v>367</v>
       </c>
@@ -4388,22 +4474,23 @@
       <c r="J61" s="12" t="s">
         <v>399</v>
       </c>
-      <c r="K61" s="34">
+      <c r="K61" s="33">
         <v>1</v>
       </c>
       <c r="L61" s="13">
         <v>12</v>
       </c>
       <c r="M61" s="16"/>
-      <c r="N61" s="16">
-        <v>1</v>
-      </c>
-      <c r="O61" s="10"/>
+      <c r="N61" s="16"/>
+      <c r="O61" s="16">
+        <v>1</v>
+      </c>
       <c r="P61" s="10"/>
-      <c r="Q61" s="11"/>
-      <c r="R61" s="11"/>
-    </row>
-    <row r="62" spans="1:18" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q61" s="10"/>
+      <c r="R61" s="29"/>
+      <c r="S61" s="28"/>
+    </row>
+    <row r="62" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="12" t="s">
         <v>367</v>
       </c>
@@ -4442,12 +4529,15 @@
       <c r="N62" s="16">
         <v>1</v>
       </c>
-      <c r="O62" s="10"/>
+      <c r="O62" s="16">
+        <v>1</v>
+      </c>
       <c r="P62" s="10"/>
-      <c r="Q62" s="11"/>
-      <c r="R62" s="11"/>
-    </row>
-    <row r="63" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q62" s="10"/>
+      <c r="R62" s="39"/>
+      <c r="S62" s="42"/>
+    </row>
+    <row r="63" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="19"/>
       <c r="B63" s="19"/>
       <c r="C63" s="19"/>
@@ -4458,16 +4548,15 @@
       <c r="H63" s="19"/>
       <c r="I63" s="19"/>
       <c r="J63" s="19"/>
-      <c r="K63" s="36"/>
-      <c r="L63" s="35"/>
+      <c r="K63" s="35"/>
+      <c r="L63" s="34"/>
       <c r="M63" s="29"/>
       <c r="N63" s="29"/>
-      <c r="O63" s="31"/>
+      <c r="O63" s="29"/>
       <c r="P63" s="31"/>
-      <c r="Q63" s="29"/>
-      <c r="R63" s="30"/>
-    </row>
-    <row r="64" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q63" s="31"/>
+    </row>
+    <row r="64" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="19"/>
       <c r="B64" s="19"/>
       <c r="C64" s="19"/>
@@ -4478,16 +4567,15 @@
       <c r="H64" s="19"/>
       <c r="I64" s="19"/>
       <c r="J64" s="19"/>
-      <c r="K64" s="36"/>
-      <c r="L64" s="35"/>
+      <c r="K64" s="35"/>
+      <c r="L64" s="34"/>
       <c r="M64" s="29"/>
       <c r="N64" s="29"/>
-      <c r="O64" s="31"/>
+      <c r="O64" s="29"/>
       <c r="P64" s="31"/>
-      <c r="Q64" s="29"/>
-      <c r="R64" s="30"/>
-    </row>
-    <row r="65" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q64" s="31"/>
+    </row>
+    <row r="65" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="19"/>
       <c r="B65" s="19"/>
       <c r="C65" s="19"/>
@@ -4498,17 +4586,17 @@
       <c r="H65" s="19"/>
       <c r="I65" s="19"/>
       <c r="J65" s="19"/>
-      <c r="K65" s="36"/>
-      <c r="L65" s="35"/>
+      <c r="K65" s="35"/>
+      <c r="L65" s="34"/>
       <c r="M65" s="29"/>
       <c r="N65" s="29"/>
-      <c r="O65" s="37"/>
-      <c r="P65" s="31"/>
-      <c r="Q65" s="29"/>
-      <c r="R65" s="28"/>
+      <c r="O65" s="29"/>
+      <c r="P65" s="36"/>
+      <c r="Q65" s="31"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="M1:N1048576">
+  <autoFilter ref="A1:O62" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="M1:O1048576">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
update post post processing process
</commit_message>
<xml_diff>
--- a/ssp_modeling/scenario_mapping/ssp_mexico_transformation_cw.xlsx
+++ b/ssp_modeling/scenario_mapping/ssp_mexico_transformation_cw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabianfuentes/git/ssp_mexico/ssp_modeling/scenario_mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7236C0-6A48-884C-9CB4-51B07503BF3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F471B6B9-6A58-A54D-8FC5-4229FE305C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-7140" windowWidth="38400" windowHeight="20980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-51200" yWindow="-7140" windowWidth="25600" windowHeight="28180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -1310,7 +1310,7 @@
     <t>magnitude_description</t>
   </si>
   <si>
-    <t>strategy_NDC+</t>
+    <t>strategy_NDC2</t>
   </si>
 </sst>
 </file>
@@ -1474,7 +1474,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1567,6 +1567,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1917,7 +1920,7 @@
   </sheetPr>
   <dimension ref="A1:S65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -1932,22 +1935,20 @@
     <col min="7" max="7" width="47.5" style="4" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="48.5" style="4" hidden="1" customWidth="1"/>
     <col min="9" max="10" width="35" style="4" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="31.5" style="38" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.83203125" style="37" customWidth="1"/>
-    <col min="13" max="13" width="20.5" style="39" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.5" style="39" customWidth="1"/>
-    <col min="15" max="15" width="20.5" style="39" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5" style="40" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.5" style="41" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.5" style="39" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.5" style="42" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.5" style="39" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.83203125" style="38" customWidth="1"/>
+    <col min="13" max="15" width="20.5" style="40" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5" style="41" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5" style="42" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.5" style="40" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.5" style="43" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="4" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="44" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -2023,8 +2024,12 @@
       <c r="L2" s="13">
         <v>12</v>
       </c>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
+      <c r="M2" s="16">
+        <v>1</v>
+      </c>
+      <c r="N2" s="16">
+        <v>1</v>
+      </c>
       <c r="O2" s="16">
         <v>1</v>
       </c>
@@ -2037,7 +2042,7 @@
       <c r="A3" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="45" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="17" t="s">
@@ -2189,7 +2194,9 @@
       </c>
       <c r="M6" s="16"/>
       <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
+      <c r="O6" s="16">
+        <v>0.1</v>
+      </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="10"/>
       <c r="R6" s="11"/>
@@ -2225,10 +2232,10 @@
         <v>12</v>
       </c>
       <c r="M7" s="16"/>
-      <c r="N7" s="16">
+      <c r="N7" s="46">
         <v>0.05</v>
       </c>
-      <c r="O7" s="45">
+      <c r="O7" s="46">
         <v>0.1</v>
       </c>
       <c r="P7" s="10"/>
@@ -2270,7 +2277,9 @@
         <v>12</v>
       </c>
       <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
+      <c r="N8" s="46">
+        <v>1</v>
+      </c>
       <c r="O8" s="16">
         <v>1</v>
       </c>
@@ -2313,7 +2322,9 @@
         <v>12</v>
       </c>
       <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
+      <c r="N9" s="46">
+        <v>1</v>
+      </c>
       <c r="O9" s="16">
         <v>1</v>
       </c>
@@ -2356,7 +2367,9 @@
         <v>12</v>
       </c>
       <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
+      <c r="N10" s="46">
+        <v>1</v>
+      </c>
       <c r="O10" s="16">
         <v>1</v>
       </c>
@@ -2395,7 +2408,7 @@
         <v>12</v>
       </c>
       <c r="M11" s="16"/>
-      <c r="N11" s="16">
+      <c r="N11" s="46">
         <v>1</v>
       </c>
       <c r="O11" s="16">
@@ -2436,7 +2449,7 @@
         <v>12</v>
       </c>
       <c r="M12" s="16"/>
-      <c r="N12" s="16">
+      <c r="N12" s="46">
         <v>1</v>
       </c>
       <c r="O12" s="16">
@@ -2483,7 +2496,7 @@
       <c r="M13" s="16">
         <v>1</v>
       </c>
-      <c r="N13" s="16">
+      <c r="N13" s="46">
         <v>1</v>
       </c>
       <c r="O13" s="16">
@@ -2528,7 +2541,9 @@
         <v>12</v>
       </c>
       <c r="M14" s="16"/>
-      <c r="N14" s="16"/>
+      <c r="N14" s="46">
+        <v>1</v>
+      </c>
       <c r="O14" s="16">
         <v>1</v>
       </c>
@@ -2567,7 +2582,9 @@
         <v>12</v>
       </c>
       <c r="M15" s="16"/>
-      <c r="N15" s="16"/>
+      <c r="N15" s="46">
+        <v>1</v>
+      </c>
       <c r="O15" s="16">
         <v>1</v>
       </c>
@@ -2856,7 +2873,7 @@
         <v>12</v>
       </c>
       <c r="M22" s="16">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N22" s="16">
         <v>1</v>
@@ -2944,7 +2961,7 @@
         <v>12</v>
       </c>
       <c r="M24" s="16">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N24" s="16">
         <v>1</v>
@@ -3267,11 +3284,13 @@
       </c>
       <c r="M32" s="16"/>
       <c r="N32" s="16"/>
-      <c r="O32" s="16"/>
+      <c r="O32" s="16">
+        <v>0.1</v>
+      </c>
       <c r="P32" s="31"/>
       <c r="Q32" s="28"/>
-      <c r="R32" s="11"/>
-      <c r="S32" s="11"/>
+      <c r="R32" s="16"/>
+      <c r="S32" s="32"/>
     </row>
     <row r="33" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
@@ -3379,7 +3398,9 @@
         <v>12</v>
       </c>
       <c r="M35" s="16"/>
-      <c r="N35" s="16"/>
+      <c r="N35" s="46">
+        <v>1</v>
+      </c>
       <c r="O35" s="16">
         <v>1</v>
       </c>
@@ -3417,8 +3438,10 @@
       <c r="L36" s="13">
         <v>12</v>
       </c>
-      <c r="M36" s="16"/>
-      <c r="N36" s="16">
+      <c r="M36" s="16">
+        <v>1</v>
+      </c>
+      <c r="N36" s="46">
         <v>1</v>
       </c>
       <c r="O36" s="16">
@@ -3459,7 +3482,9 @@
         <v>12</v>
       </c>
       <c r="M37" s="16"/>
-      <c r="N37" s="16"/>
+      <c r="N37" s="46">
+        <v>1</v>
+      </c>
       <c r="O37" s="16">
         <v>1</v>
       </c>
@@ -3498,7 +3523,9 @@
         <v>12</v>
       </c>
       <c r="M38" s="16"/>
-      <c r="N38" s="16"/>
+      <c r="N38" s="16">
+        <v>1</v>
+      </c>
       <c r="O38" s="16">
         <v>1</v>
       </c>
@@ -3583,12 +3610,14 @@
       <c r="L40" s="13">
         <v>12</v>
       </c>
-      <c r="M40" s="16"/>
-      <c r="N40" s="16">
+      <c r="M40" s="16">
+        <v>1</v>
+      </c>
+      <c r="N40" s="46">
         <v>1</v>
       </c>
       <c r="O40" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P40" s="10"/>
       <c r="Q40" s="10"/>
@@ -3615,7 +3644,7 @@
         <v>327</v>
       </c>
       <c r="G41" s="12"/>
-      <c r="H41" s="32"/>
+      <c r="H41" s="33"/>
       <c r="I41" s="12" t="s">
         <v>328</v>
       </c>
@@ -3629,9 +3658,11 @@
         <v>12</v>
       </c>
       <c r="M41" s="16"/>
-      <c r="N41" s="16"/>
+      <c r="N41" s="46">
+        <v>1</v>
+      </c>
       <c r="O41" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P41" s="10"/>
       <c r="Q41" s="10"/>
@@ -3658,7 +3689,7 @@
         <v>331</v>
       </c>
       <c r="G42" s="12"/>
-      <c r="H42" s="32"/>
+      <c r="H42" s="33"/>
       <c r="I42" s="12" t="s">
         <v>332</v>
       </c>
@@ -3672,9 +3703,11 @@
         <v>12</v>
       </c>
       <c r="M42" s="16"/>
-      <c r="N42" s="16"/>
+      <c r="N42" s="46">
+        <v>1</v>
+      </c>
       <c r="O42" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P42" s="10"/>
       <c r="Q42" s="10"/>
@@ -3711,9 +3744,11 @@
         <v>12</v>
       </c>
       <c r="M43" s="16"/>
-      <c r="N43" s="16"/>
+      <c r="N43" s="46">
+        <v>1</v>
+      </c>
       <c r="O43" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P43" s="10"/>
       <c r="Q43" s="10"/>
@@ -3752,7 +3787,7 @@
       <c r="M44" s="16">
         <v>1</v>
       </c>
-      <c r="N44" s="16">
+      <c r="N44" s="46">
         <v>1</v>
       </c>
       <c r="O44" s="16">
@@ -3797,7 +3832,9 @@
         <v>12</v>
       </c>
       <c r="M45" s="16"/>
-      <c r="N45" s="16"/>
+      <c r="N45" s="46">
+        <v>1</v>
+      </c>
       <c r="O45" s="16">
         <v>1</v>
       </c>
@@ -3842,7 +3879,7 @@
       <c r="M46" s="16">
         <v>1</v>
       </c>
-      <c r="N46" s="16">
+      <c r="N46" s="46">
         <v>1</v>
       </c>
       <c r="O46" s="16">
@@ -3885,11 +3922,11 @@
       <c r="M47" s="16">
         <v>1</v>
       </c>
-      <c r="N47" s="16">
+      <c r="N47" s="46">
         <v>1</v>
       </c>
       <c r="O47" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P47" s="10"/>
       <c r="Q47" s="10"/>
@@ -3932,11 +3969,11 @@
       <c r="M48" s="16">
         <v>1</v>
       </c>
-      <c r="N48" s="16">
+      <c r="N48" s="46">
         <v>1</v>
       </c>
       <c r="O48" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P48" s="10"/>
       <c r="Q48" s="10"/>
@@ -3979,11 +4016,11 @@
       <c r="M49" s="16">
         <v>1</v>
       </c>
-      <c r="N49" s="16">
+      <c r="N49" s="46">
         <v>1</v>
       </c>
       <c r="O49" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P49" s="10"/>
       <c r="Q49" s="10"/>
@@ -4024,7 +4061,9 @@
         <v>12</v>
       </c>
       <c r="M50" s="16"/>
-      <c r="N50" s="16"/>
+      <c r="N50" s="46">
+        <v>1</v>
+      </c>
       <c r="O50" s="16">
         <v>1</v>
       </c>
@@ -4151,7 +4190,7 @@
       <c r="M53" s="16"/>
       <c r="N53" s="16"/>
       <c r="O53" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P53" s="10"/>
       <c r="Q53" s="10"/>
@@ -4405,8 +4444,8 @@
       </c>
       <c r="P59" s="10"/>
       <c r="Q59" s="10"/>
-      <c r="R59" s="29"/>
-      <c r="S59" s="30"/>
+      <c r="R59" s="11"/>
+      <c r="S59" s="11"/>
     </row>
     <row r="60" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="12" t="s">
@@ -4444,8 +4483,8 @@
       </c>
       <c r="P60" s="10"/>
       <c r="Q60" s="10"/>
-      <c r="R60" s="29"/>
-      <c r="S60" s="30"/>
+      <c r="R60" s="11"/>
+      <c r="S60" s="11"/>
     </row>
     <row r="61" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="12" t="s">
@@ -4474,7 +4513,7 @@
       <c r="J61" s="12" t="s">
         <v>399</v>
       </c>
-      <c r="K61" s="33">
+      <c r="K61" s="34">
         <v>1</v>
       </c>
       <c r="L61" s="13">
@@ -4487,8 +4526,8 @@
       </c>
       <c r="P61" s="10"/>
       <c r="Q61" s="10"/>
-      <c r="R61" s="29"/>
-      <c r="S61" s="28"/>
+      <c r="R61" s="11"/>
+      <c r="S61" s="11"/>
     </row>
     <row r="62" spans="1:19" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="12" t="s">
@@ -4534,8 +4573,8 @@
       </c>
       <c r="P62" s="10"/>
       <c r="Q62" s="10"/>
-      <c r="R62" s="39"/>
-      <c r="S62" s="42"/>
+      <c r="R62" s="11"/>
+      <c r="S62" s="11"/>
     </row>
     <row r="63" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="19"/>
@@ -4548,13 +4587,15 @@
       <c r="H63" s="19"/>
       <c r="I63" s="19"/>
       <c r="J63" s="19"/>
-      <c r="K63" s="35"/>
-      <c r="L63" s="34"/>
+      <c r="K63" s="36"/>
+      <c r="L63" s="35"/>
       <c r="M63" s="29"/>
       <c r="N63" s="29"/>
       <c r="O63" s="29"/>
       <c r="P63" s="31"/>
       <c r="Q63" s="31"/>
+      <c r="R63" s="29"/>
+      <c r="S63" s="30"/>
     </row>
     <row r="64" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="19"/>
@@ -4567,15 +4608,17 @@
       <c r="H64" s="19"/>
       <c r="I64" s="19"/>
       <c r="J64" s="19"/>
-      <c r="K64" s="35"/>
-      <c r="L64" s="34"/>
+      <c r="K64" s="36"/>
+      <c r="L64" s="35"/>
       <c r="M64" s="29"/>
       <c r="N64" s="29"/>
       <c r="O64" s="29"/>
       <c r="P64" s="31"/>
       <c r="Q64" s="31"/>
-    </row>
-    <row r="65" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R64" s="29"/>
+      <c r="S64" s="30"/>
+    </row>
+    <row r="65" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="19"/>
       <c r="B65" s="19"/>
       <c r="C65" s="19"/>
@@ -4586,17 +4629,31 @@
       <c r="H65" s="19"/>
       <c r="I65" s="19"/>
       <c r="J65" s="19"/>
-      <c r="K65" s="35"/>
-      <c r="L65" s="34"/>
+      <c r="K65" s="36"/>
+      <c r="L65" s="35"/>
       <c r="M65" s="29"/>
       <c r="N65" s="29"/>
       <c r="O65" s="29"/>
-      <c r="P65" s="36"/>
+      <c r="P65" s="37"/>
       <c r="Q65" s="31"/>
+      <c r="R65" s="29"/>
+      <c r="S65" s="28"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:O62" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="M1:O1048576">
+  <conditionalFormatting sqref="M1:O39 M40:N40 M41:O1048576">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O40">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>